<commit_message>
updated training results excel sheet
</commit_message>
<xml_diff>
--- a/train_results.xlsx
+++ b/train_results.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raphael\polymtl\deep_learning\DL_Ass2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8FD17463-70CE-446E-9DED-C6C6949EC79D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4150CECF-A651-4622-92E5-C2AB2188BCB8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{B40B11C7-0A3F-4D0E-9D63-29A1301B19CB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="95">
   <si>
     <t>GRU_ADAM</t>
   </si>
@@ -59,33 +59,6 @@
     <t>102.47938350406689</t>
   </si>
   <si>
-    <t>GRU_SGD_LR_SCHEDULE_HIDDENSIZE_2200</t>
-  </si>
-  <si>
-    <t>57.50682219208625</t>
-  </si>
-  <si>
-    <t>104.03431814057733</t>
-  </si>
-  <si>
-    <t>GRU_SGD_LR_SCHEDULE_NUMLAYERS_3</t>
-  </si>
-  <si>
-    <t>75.90899430466085</t>
-  </si>
-  <si>
-    <t>111.8298056434746</t>
-  </si>
-  <si>
-    <t>GRU_SGD_LR_SCHEDULE_SEQLEN_50</t>
-  </si>
-  <si>
-    <t>67.93366456217746</t>
-  </si>
-  <si>
-    <t>103.07147912894796</t>
-  </si>
-  <si>
     <t>RNN_ADAM</t>
   </si>
   <si>
@@ -113,21 +86,251 @@
     <t>196.42214767910397</t>
   </si>
   <si>
-    <t>Experience name</t>
-  </si>
-  <si>
-    <t>train ppl</t>
-  </si>
-  <si>
-    <t>val ppl</t>
+    <t>0.35</t>
+  </si>
+  <si>
+    <t>0.0001</t>
+  </si>
+  <si>
+    <t>GRU</t>
+  </si>
+  <si>
+    <t>ADAM</t>
+  </si>
+  <si>
+    <t>GRU_random_hyperparameters_best</t>
+  </si>
+  <si>
+    <t>0.34099590627753534</t>
+  </si>
+  <si>
+    <t>13.187674054337151</t>
+  </si>
+  <si>
+    <t>SGD_LR_SCHEDULE</t>
+  </si>
+  <si>
+    <t>65.52871900673708</t>
+  </si>
+  <si>
+    <t>93.38046491546288</t>
+  </si>
+  <si>
+    <t>GRU_random_hyperparameters_better_1</t>
+  </si>
+  <si>
+    <t>0.4939787146651825</t>
+  </si>
+  <si>
+    <t>8.562059059815436</t>
+  </si>
+  <si>
+    <t>67.2384852045134</t>
+  </si>
+  <si>
+    <t>97.44802989256516</t>
+  </si>
+  <si>
+    <t>GRU_random_hyperparameters_better_2</t>
+  </si>
+  <si>
+    <t>0.33987809307704897</t>
+  </si>
+  <si>
+    <t>7.645957899852757</t>
+  </si>
+  <si>
+    <t>68.22335469573727</t>
+  </si>
+  <si>
+    <t>97.74139617454416</t>
+  </si>
+  <si>
+    <t>10.0</t>
+  </si>
+  <si>
+    <t>SGD</t>
+  </si>
+  <si>
+    <t>RNN</t>
+  </si>
+  <si>
+    <t>RNN_random_hyperparameters_best</t>
+  </si>
+  <si>
+    <t>0.4415538384431265</t>
+  </si>
+  <si>
+    <t>0.00011005411679699441</t>
+  </si>
+  <si>
+    <t>101.78762282075765</t>
+  </si>
+  <si>
+    <t>139.42743787410262</t>
+  </si>
+  <si>
+    <t>RNN_random_hyperparameters_better_1</t>
+  </si>
+  <si>
+    <t>0.49012323313650574</t>
+  </si>
+  <si>
+    <t>0.00010983768204457021</t>
+  </si>
+  <si>
+    <t>99.48660016245752</t>
+  </si>
+  <si>
+    <t>150.43841562588528</t>
+  </si>
+  <si>
+    <t>RNN_random_hyperparameters_better_2</t>
+  </si>
+  <si>
+    <t>0.4384916082357852</t>
+  </si>
+  <si>
+    <t>6.34747636016373e-05</t>
+  </si>
+  <si>
+    <t>98.64935974536745</t>
+  </si>
+  <si>
+    <t>140.02971530726305</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>TRANSFORMER_ADAM</t>
+  </si>
+  <si>
+    <t>0.9</t>
+  </si>
+  <si>
+    <t>0.001</t>
+  </si>
+  <si>
+    <t>TRANSFORMER</t>
+  </si>
+  <si>
+    <t>TRANSFORMER_SGD</t>
+  </si>
+  <si>
+    <t>20.0</t>
+  </si>
+  <si>
+    <t>TRANSFORMER_SGD_LR_SCHEDULE</t>
+  </si>
+  <si>
+    <t>batch_size</t>
+  </si>
+  <si>
+    <t>dp_keep_prob</t>
+  </si>
+  <si>
+    <t>emb_size</t>
+  </si>
+  <si>
+    <t>hidden_size</t>
+  </si>
+  <si>
+    <t>initial_lr</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>num_layers</t>
+  </si>
+  <si>
+    <t>optimizer</t>
+  </si>
+  <si>
+    <t>seq_len</t>
+  </si>
+  <si>
+    <t>train_ppl</t>
+  </si>
+  <si>
+    <t>val_ppl</t>
+  </si>
+  <si>
+    <t>94.15780121166866</t>
+  </si>
+  <si>
+    <t>136.8132423763601</t>
+  </si>
+  <si>
+    <t>TRANSFORMER_random_hyperparameters_best</t>
+  </si>
+  <si>
+    <t>0.0006805458932727954</t>
+  </si>
+  <si>
+    <t>74.13083852763428</t>
+  </si>
+  <si>
+    <t>129.69166756532726</t>
+  </si>
+  <si>
+    <t>TRANSFORMER_random_hyperparameters_better_1</t>
+  </si>
+  <si>
+    <t>0.0008641222122005982</t>
+  </si>
+  <si>
+    <t>76.08358106085699</t>
+  </si>
+  <si>
+    <t>130.98787805201212</t>
+  </si>
+  <si>
+    <t>TRANSFORMER_random_hyperparameters_better_2</t>
+  </si>
+  <si>
+    <t>0.0010429422250618418</t>
+  </si>
+  <si>
+    <t>74.47834228498705</t>
+  </si>
+  <si>
+    <t>132.8694970700487</t>
+  </si>
+  <si>
+    <t>80.59542483617577</t>
+  </si>
+  <si>
+    <t>168.2985398732332</t>
+  </si>
+  <si>
+    <t>57.75553490589902</t>
+  </si>
+  <si>
+    <t>147.94945961372298</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -155,8 +358,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,130 +674,808 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0892D55C-040B-4401-A16D-D34FC79611C7}">
-  <dimension ref="A1:C10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8755BC41-A42C-40DB-9C04-80B6909A9396}">
+  <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2">
+        <v>200</v>
+      </c>
+      <c r="H2">
+        <v>1500</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <v>35</v>
+      </c>
+      <c r="L2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="1">
+        <v>25</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="1">
+        <v>220</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1186</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1</v>
+      </c>
+      <c r="K3" s="1">
         <v>27</v>
       </c>
-      <c r="B1" t="s">
+      <c r="L3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>28</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="G4">
+        <v>286</v>
+      </c>
+      <c r="H4">
+        <v>482</v>
+      </c>
+      <c r="I4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <v>12</v>
+      </c>
+      <c r="L4" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5">
+        <v>322</v>
+      </c>
+      <c r="H5">
+        <v>1798</v>
+      </c>
+      <c r="I5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="K5">
+        <v>47</v>
+      </c>
+      <c r="L5" t="s">
+        <v>36</v>
+      </c>
+      <c r="M5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6">
+        <v>200</v>
+      </c>
+      <c r="H6">
+        <v>1500</v>
+      </c>
+      <c r="I6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="K6">
+        <v>35</v>
+      </c>
+      <c r="L6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="M6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7">
+        <v>20</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7">
+        <v>200</v>
+      </c>
+      <c r="H7">
+        <v>1500</v>
+      </c>
+      <c r="I7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <v>35</v>
+      </c>
+      <c r="L7" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="M7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8">
+        <v>20</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8">
+        <v>200</v>
+      </c>
+      <c r="H8">
+        <v>1500</v>
+      </c>
+      <c r="I8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8">
+        <v>2</v>
+      </c>
+      <c r="K8">
+        <v>35</v>
+      </c>
+      <c r="L8" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
+      <c r="M8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="9" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="1">
+        <v>20</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="1">
+        <v>474</v>
+      </c>
+      <c r="H9" s="1">
+        <v>1314</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J9" s="1">
+        <v>2</v>
+      </c>
+      <c r="K9" s="1">
+        <v>37</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10">
+        <v>15</v>
+      </c>
+      <c r="F10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10">
+        <v>323</v>
+      </c>
+      <c r="H10">
+        <v>1386</v>
+      </c>
+      <c r="I10" t="s">
+        <v>48</v>
+      </c>
+      <c r="J10">
+        <v>2</v>
+      </c>
+      <c r="K10">
+        <v>28</v>
+      </c>
+      <c r="L10" t="s">
+        <v>49</v>
+      </c>
+      <c r="M10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11">
+        <v>19</v>
+      </c>
+      <c r="F11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11">
+        <v>333</v>
+      </c>
+      <c r="H11">
+        <v>1126</v>
+      </c>
+      <c r="I11" t="s">
+        <v>53</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>25</v>
+      </c>
+      <c r="L11" t="s">
+        <v>54</v>
+      </c>
+      <c r="M11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12">
+        <v>20</v>
+      </c>
+      <c r="F12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12">
+        <v>200</v>
+      </c>
+      <c r="H12">
+        <v>1500</v>
+      </c>
+      <c r="I12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12">
+        <v>2</v>
+      </c>
+      <c r="K12">
+        <v>35</v>
+      </c>
+      <c r="L12" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
+      <c r="M12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13">
+        <v>20</v>
+      </c>
+      <c r="F13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13">
+        <v>200</v>
+      </c>
+      <c r="H13">
+        <v>512</v>
+      </c>
+      <c r="I13" t="s">
+        <v>56</v>
+      </c>
+      <c r="J13">
+        <v>2</v>
+      </c>
+      <c r="K13">
+        <v>35</v>
+      </c>
+      <c r="L13" t="s">
         <v>16</v>
       </c>
-      <c r="C7" t="s">
+      <c r="M13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14">
+        <v>128</v>
+      </c>
+      <c r="F14" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14">
+        <v>200</v>
+      </c>
+      <c r="H14">
+        <v>512</v>
+      </c>
+      <c r="I14" t="s">
+        <v>59</v>
+      </c>
+      <c r="J14">
+        <v>2</v>
+      </c>
+      <c r="K14">
+        <v>35</v>
+      </c>
+      <c r="L14" t="s">
+        <v>75</v>
+      </c>
+      <c r="M14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="1">
+        <v>156</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15" s="1">
+        <v>273</v>
+      </c>
+      <c r="H15" s="1">
+        <v>608</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J15" s="1">
+        <v>2</v>
+      </c>
+      <c r="K15" s="1">
+        <v>45</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16">
+        <v>135</v>
+      </c>
+      <c r="F16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G16">
+        <v>202</v>
+      </c>
+      <c r="H16">
+        <v>416</v>
+      </c>
+      <c r="I16" t="s">
+        <v>82</v>
+      </c>
+      <c r="J16">
+        <v>2</v>
+      </c>
+      <c r="K16">
+        <v>34</v>
+      </c>
+      <c r="L16" t="s">
+        <v>83</v>
+      </c>
+      <c r="M16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17">
+        <v>89</v>
+      </c>
+      <c r="F17" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17">
+        <v>293</v>
+      </c>
+      <c r="H17">
+        <v>384</v>
+      </c>
+      <c r="I17" t="s">
+        <v>86</v>
+      </c>
+      <c r="J17">
+        <v>2</v>
+      </c>
+      <c r="K17">
+        <v>45</v>
+      </c>
+      <c r="L17" t="s">
+        <v>87</v>
+      </c>
+      <c r="M17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18">
+        <v>128</v>
+      </c>
+      <c r="F18" t="s">
+        <v>58</v>
+      </c>
+      <c r="G18">
+        <v>200</v>
+      </c>
+      <c r="H18">
+        <v>512</v>
+      </c>
+      <c r="I18" t="s">
+        <v>62</v>
+      </c>
+      <c r="J18">
+        <v>6</v>
+      </c>
+      <c r="K18">
+        <v>35</v>
+      </c>
+      <c r="L18" t="s">
+        <v>89</v>
+      </c>
+      <c r="M18" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19">
         <v>18</v>
       </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="B19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" t="s">
         <v>25</v>
       </c>
-      <c r="C10" t="s">
-        <v>26</v>
+      <c r="E19">
+        <v>128</v>
+      </c>
+      <c r="F19" t="s">
+        <v>58</v>
+      </c>
+      <c r="G19">
+        <v>200</v>
+      </c>
+      <c r="H19">
+        <v>512</v>
+      </c>
+      <c r="I19" t="s">
+        <v>62</v>
+      </c>
+      <c r="J19">
+        <v>6</v>
+      </c>
+      <c r="K19">
+        <v>35</v>
+      </c>
+      <c r="L19" t="s">
+        <v>91</v>
+      </c>
+      <c r="M19" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated visual of excel sheet and created an image with it
</commit_message>
<xml_diff>
--- a/train_results.xlsx
+++ b/train_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raphael\polymtl\deep_learning\DL_Ass2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4150CECF-A651-4622-92E5-C2AB2188BCB8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E74A77-EC4D-433D-A335-7D230371EF79}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{B40B11C7-0A3F-4D0E-9D63-29A1301B19CB}"/>
   </bookViews>
@@ -376,6 +376,42 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9A367BF3-ABB1-43D0-B304-F5CDA1BA5AD5}" name="Table3" displayName="Table3" ref="A1:M19">
+  <autoFilter ref="A1:M19" xr:uid="{AE830C7A-34A0-443D-861F-795808C4114D}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+    <filterColumn colId="7" hiddenButton="1"/>
+    <filterColumn colId="8" hiddenButton="1"/>
+    <filterColumn colId="9" hiddenButton="1"/>
+    <filterColumn colId="10" hiddenButton="1"/>
+    <filterColumn colId="11" hiddenButton="1"/>
+    <filterColumn colId="12" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{B51EA972-A26B-4F2D-A775-AC4C813C7D45}" name="id" totalsRowLabel="Total"/>
+    <tableColumn id="2" xr3:uid="{DE189E54-A651-42F8-A6AB-FAAC66B76417}" name="name"/>
+    <tableColumn id="3" xr3:uid="{EEA6F7F3-A61A-43F6-9CB6-CCAA72896CB4}" name="model"/>
+    <tableColumn id="4" xr3:uid="{3A2E272D-F6EF-47D0-9E71-A87987C1BC59}" name="optimizer"/>
+    <tableColumn id="5" xr3:uid="{1028DA1F-BF99-4F6A-A422-37A366ABDEEF}" name="batch_size"/>
+    <tableColumn id="6" xr3:uid="{0AF341D3-7CC0-42E3-A8BC-CDC1C29EFBCC}" name="dp_keep_prob"/>
+    <tableColumn id="7" xr3:uid="{0D363AC1-9D63-40B4-8A66-FC2FD25D54EF}" name="emb_size"/>
+    <tableColumn id="8" xr3:uid="{5F1AB3CA-49CA-4F6D-B7B7-13CA4D8D56EE}" name="hidden_size"/>
+    <tableColumn id="9" xr3:uid="{FCD73196-6C9E-4181-928D-2A7492361D36}" name="initial_lr"/>
+    <tableColumn id="10" xr3:uid="{AF23CC4E-9234-4A4E-96A4-864D7FCDE37A}" name="num_layers"/>
+    <tableColumn id="11" xr3:uid="{5649DAE7-CFF0-4DE9-9587-D2E061CCFC7D}" name="seq_len"/>
+    <tableColumn id="12" xr3:uid="{D5EA2D03-017D-4F6C-B143-2DF45B6BB0CA}" name="train_ppl"/>
+    <tableColumn id="13" xr3:uid="{0626AB2B-DD7F-4FF1-9392-F05BDC768D76}" name="val_ppl" totalsRowFunction="count"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -678,21 +714,22 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="44.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.6640625" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" customWidth="1"/>
     <col min="6" max="6" width="19.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" customWidth="1"/>
     <col min="9" max="9" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.21875" customWidth="1"/>
+    <col min="11" max="11" width="9.109375" customWidth="1"/>
+    <col min="12" max="13" width="18.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
@@ -1477,5 +1514,8 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated plot script and results
</commit_message>
<xml_diff>
--- a/train_results.xlsx
+++ b/train_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raphael\polymtl\deep_learning\DL_Ass2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E74A77-EC4D-433D-A335-7D230371EF79}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD15FC0F-F965-4460-AD4A-664DD67B1244}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{B40B11C7-0A3F-4D0E-9D63-29A1301B19CB}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="90">
   <si>
     <t>GRU_ADAM</t>
   </si>
@@ -101,12 +101,6 @@
     <t>GRU_random_hyperparameters_best</t>
   </si>
   <si>
-    <t>0.34099590627753534</t>
-  </si>
-  <si>
-    <t>13.187674054337151</t>
-  </si>
-  <si>
     <t>SGD_LR_SCHEDULE</t>
   </si>
   <si>
@@ -119,12 +113,6 @@
     <t>GRU_random_hyperparameters_better_1</t>
   </si>
   <si>
-    <t>0.4939787146651825</t>
-  </si>
-  <si>
-    <t>8.562059059815436</t>
-  </si>
-  <si>
     <t>67.2384852045134</t>
   </si>
   <si>
@@ -134,12 +122,6 @@
     <t>GRU_random_hyperparameters_better_2</t>
   </si>
   <si>
-    <t>0.33987809307704897</t>
-  </si>
-  <si>
-    <t>7.645957899852757</t>
-  </si>
-  <si>
     <t>68.22335469573727</t>
   </si>
   <si>
@@ -158,12 +140,6 @@
     <t>RNN_random_hyperparameters_best</t>
   </si>
   <si>
-    <t>0.4415538384431265</t>
-  </si>
-  <si>
-    <t>0.00011005411679699441</t>
-  </si>
-  <si>
     <t>101.78762282075765</t>
   </si>
   <si>
@@ -173,12 +149,6 @@
     <t>RNN_random_hyperparameters_better_1</t>
   </si>
   <si>
-    <t>0.49012323313650574</t>
-  </si>
-  <si>
-    <t>0.00010983768204457021</t>
-  </si>
-  <si>
     <t>99.48660016245752</t>
   </si>
   <si>
@@ -188,12 +158,6 @@
     <t>RNN_random_hyperparameters_better_2</t>
   </si>
   <si>
-    <t>0.4384916082357852</t>
-  </si>
-  <si>
-    <t>6.34747636016373e-05</t>
-  </si>
-  <si>
     <t>98.64935974536745</t>
   </si>
   <si>
@@ -266,9 +230,6 @@
     <t>TRANSFORMER_random_hyperparameters_best</t>
   </si>
   <si>
-    <t>0.0006805458932727954</t>
-  </si>
-  <si>
     <t>74.13083852763428</t>
   </si>
   <si>
@@ -278,9 +239,6 @@
     <t>TRANSFORMER_random_hyperparameters_better_1</t>
   </si>
   <si>
-    <t>0.0008641222122005982</t>
-  </si>
-  <si>
     <t>76.08358106085699</t>
   </si>
   <si>
@@ -290,15 +248,6 @@
     <t>TRANSFORMER_random_hyperparameters_better_2</t>
   </si>
   <si>
-    <t>0.0010429422250618418</t>
-  </si>
-  <si>
-    <t>74.47834228498705</t>
-  </si>
-  <si>
-    <t>132.8694970700487</t>
-  </si>
-  <si>
     <t>80.59542483617577</t>
   </si>
   <si>
@@ -315,13 +264,53 @@
   </si>
   <si>
     <t>name</t>
+  </si>
+  <si>
+    <t>0.8</t>
+  </si>
+  <si>
+    <t>56.040139934093375</t>
+  </si>
+  <si>
+    <t>120.5052039280884</t>
+  </si>
+  <si>
+    <t>0.34</t>
+  </si>
+  <si>
+    <t>0.49</t>
+  </si>
+  <si>
+    <t>0.44</t>
+  </si>
+  <si>
+    <t>13.188</t>
+  </si>
+  <si>
+    <t>8.562</t>
+  </si>
+  <si>
+    <t>7.646</t>
+  </si>
+  <si>
+    <t>0.00006</t>
+  </si>
+  <si>
+    <t>0.0007</t>
+  </si>
+  <si>
+    <t>0.0009</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_)\ _$_ ;_ * \(#,##0.00\)\ _$_ ;_ * &quot;-&quot;??_)\ _$_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -337,16 +326,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -354,18 +356,69 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -401,14 +454,18 @@
     <tableColumn id="3" xr3:uid="{EEA6F7F3-A61A-43F6-9CB6-CCAA72896CB4}" name="model"/>
     <tableColumn id="4" xr3:uid="{3A2E272D-F6EF-47D0-9E71-A87987C1BC59}" name="optimizer"/>
     <tableColumn id="5" xr3:uid="{1028DA1F-BF99-4F6A-A422-37A366ABDEEF}" name="batch_size"/>
-    <tableColumn id="6" xr3:uid="{0AF341D3-7CC0-42E3-A8BC-CDC1C29EFBCC}" name="dp_keep_prob"/>
+    <tableColumn id="6" xr3:uid="{0AF341D3-7CC0-42E3-A8BC-CDC1C29EFBCC}" name="dp_keep_prob" dataDxfId="2"/>
     <tableColumn id="7" xr3:uid="{0D363AC1-9D63-40B4-8A66-FC2FD25D54EF}" name="emb_size"/>
     <tableColumn id="8" xr3:uid="{5F1AB3CA-49CA-4F6D-B7B7-13CA4D8D56EE}" name="hidden_size"/>
     <tableColumn id="9" xr3:uid="{FCD73196-6C9E-4181-928D-2A7492361D36}" name="initial_lr"/>
     <tableColumn id="10" xr3:uid="{AF23CC4E-9234-4A4E-96A4-864D7FCDE37A}" name="num_layers"/>
     <tableColumn id="11" xr3:uid="{5649DAE7-CFF0-4DE9-9587-D2E061CCFC7D}" name="seq_len"/>
-    <tableColumn id="12" xr3:uid="{D5EA2D03-017D-4F6C-B143-2DF45B6BB0CA}" name="train_ppl"/>
-    <tableColumn id="13" xr3:uid="{0626AB2B-DD7F-4FF1-9392-F05BDC768D76}" name="val_ppl" totalsRowFunction="count"/>
+    <tableColumn id="12" xr3:uid="{D5EA2D03-017D-4F6C-B143-2DF45B6BB0CA}" name="train_ppl" dataDxfId="1">
+      <calculatedColumnFormula>ROUND(O2,1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="13" xr3:uid="{0626AB2B-DD7F-4FF1-9392-F05BDC768D76}" name="val_ppl" totalsRowFunction="count" dataDxfId="0">
+      <calculatedColumnFormula>ROUND(P2,1)</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -711,10 +768,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8755BC41-A42C-40DB-9C04-80B6909A9396}">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -722,58 +779,59 @@
     <col min="2" max="2" width="44.6640625" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.44140625" customWidth="1"/>
     <col min="8" max="8" width="12.33203125" customWidth="1"/>
-    <col min="9" max="9" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.21875" customWidth="1"/>
     <col min="11" max="11" width="9.109375" customWidth="1"/>
-    <col min="12" max="13" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.109375" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="B1" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="C1" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="D1" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="E1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F1" t="s">
-        <v>65</v>
+        <v>52</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>53</v>
       </c>
       <c r="G1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="H1" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="I1" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="J1" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="K1" t="s">
-        <v>72</v>
-      </c>
-      <c r="L1" t="s">
-        <v>73</v>
-      </c>
-      <c r="M1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -789,7 +847,7 @@
       <c r="E2">
         <v>20</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="9" t="s">
         <v>18</v>
       </c>
       <c r="G2">
@@ -807,178 +865,218 @@
       <c r="K2">
         <v>35</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="7">
+        <f>ROUND(O2,1)</f>
+        <v>79.7</v>
+      </c>
+      <c r="M2" s="7">
+        <f>ROUND(P2,1)</f>
+        <v>112.4</v>
+      </c>
+      <c r="O2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="M2" t="s">
+      <c r="P2" s="12" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3">
+        <v>200</v>
+      </c>
+      <c r="H3">
+        <v>1500</v>
+      </c>
+      <c r="I3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>35</v>
+      </c>
+      <c r="L3" s="7">
+        <f t="shared" ref="L3:L19" si="0">ROUND(O3,1)</f>
+        <v>63.7</v>
+      </c>
+      <c r="M3" s="7">
+        <f t="shared" ref="M3:M19" si="1">ROUND(P3,1)</f>
+        <v>111.8</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="P3" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="1">
         <v>25</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F4" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="G4" s="1">
+        <v>220</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1186</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1">
+        <v>27</v>
+      </c>
+      <c r="L4" s="8">
+        <f t="shared" si="0"/>
+        <v>65.5</v>
+      </c>
+      <c r="M4" s="8">
+        <f t="shared" si="1"/>
+        <v>93.4</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="1">
-        <v>220</v>
-      </c>
-      <c r="H3" s="1">
-        <v>1186</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" s="1">
-        <v>1</v>
-      </c>
-      <c r="K3" s="1">
-        <v>27</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4">
-        <v>20</v>
-      </c>
-      <c r="F4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4">
-        <v>286</v>
-      </c>
-      <c r="H4">
-        <v>482</v>
-      </c>
-      <c r="I4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4">
-        <v>2</v>
-      </c>
-      <c r="K4">
-        <v>12</v>
-      </c>
-      <c r="L4" t="s">
-        <v>31</v>
-      </c>
-      <c r="M4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E5">
-        <v>32</v>
-      </c>
-      <c r="F5" t="s">
-        <v>34</v>
+        <v>20</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>82</v>
       </c>
       <c r="G5">
-        <v>322</v>
+        <v>286</v>
       </c>
       <c r="H5">
-        <v>1798</v>
+        <v>482</v>
       </c>
       <c r="I5" t="s">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K5">
-        <v>47</v>
-      </c>
-      <c r="L5" t="s">
-        <v>36</v>
-      </c>
-      <c r="M5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="L5" s="7">
+        <f t="shared" si="0"/>
+        <v>67.2</v>
+      </c>
+      <c r="M5" s="7">
+        <f t="shared" si="1"/>
+        <v>97.4</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P5" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
         <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="E6">
-        <v>20</v>
-      </c>
-      <c r="F6" t="s">
-        <v>18</v>
+        <v>32</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="G6">
-        <v>200</v>
+        <v>322</v>
       </c>
       <c r="H6">
-        <v>1500</v>
+        <v>1798</v>
       </c>
       <c r="I6" t="s">
-        <v>38</v>
+        <v>86</v>
       </c>
       <c r="J6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K6">
-        <v>35</v>
-      </c>
-      <c r="L6" t="s">
-        <v>4</v>
-      </c>
-      <c r="M6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+      <c r="L6" s="7">
+        <f t="shared" si="0"/>
+        <v>68.2</v>
+      </c>
+      <c r="M6" s="7">
+        <f t="shared" si="1"/>
+        <v>97.7</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="P6" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -989,12 +1087,12 @@
         <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E7">
         <v>20</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="9" t="s">
         <v>18</v>
       </c>
       <c r="G7">
@@ -1004,7 +1102,7 @@
         <v>1500</v>
       </c>
       <c r="I7" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="J7">
         <v>2</v>
@@ -1012,14 +1110,22 @@
       <c r="K7">
         <v>35</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" s="7">
+        <f t="shared" si="0"/>
+        <v>65.599999999999994</v>
+      </c>
+      <c r="M7" s="7">
+        <f t="shared" si="1"/>
+        <v>102.5</v>
+      </c>
+      <c r="O7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="M7" t="s">
+      <c r="P7" s="13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1027,7 +1133,7 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
@@ -1035,7 +1141,7 @@
       <c r="E8">
         <v>20</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="9" t="s">
         <v>18</v>
       </c>
       <c r="G8">
@@ -1053,22 +1159,30 @@
       <c r="K8">
         <v>35</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" s="7">
+        <f t="shared" si="0"/>
+        <v>128.69999999999999</v>
+      </c>
+      <c r="M8" s="7">
+        <f t="shared" si="1"/>
+        <v>156.80000000000001</v>
+      </c>
+      <c r="O8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M8" t="s">
+      <c r="P8" s="12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>21</v>
@@ -1076,8 +1190,8 @@
       <c r="E9" s="1">
         <v>20</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>42</v>
+      <c r="F9" s="10" t="s">
+        <v>83</v>
       </c>
       <c r="G9" s="1">
         <v>474</v>
@@ -1086,7 +1200,7 @@
         <v>1314</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="J9" s="1">
         <v>2</v>
@@ -1094,22 +1208,30 @@
       <c r="K9" s="1">
         <v>37</v>
       </c>
-      <c r="L9" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L9" s="8">
+        <f t="shared" si="0"/>
+        <v>101.8</v>
+      </c>
+      <c r="M9" s="8">
+        <f t="shared" si="1"/>
+        <v>139.4</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="P9" s="15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
         <v>21</v>
@@ -1117,8 +1239,8 @@
       <c r="E10">
         <v>15</v>
       </c>
-      <c r="F10" t="s">
-        <v>47</v>
+      <c r="F10" s="9" t="s">
+        <v>82</v>
       </c>
       <c r="G10">
         <v>323</v>
@@ -1127,7 +1249,7 @@
         <v>1386</v>
       </c>
       <c r="I10" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="J10">
         <v>2</v>
@@ -1135,22 +1257,30 @@
       <c r="K10">
         <v>28</v>
       </c>
-      <c r="L10" t="s">
-        <v>49</v>
-      </c>
-      <c r="M10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L10" s="7">
+        <f t="shared" si="0"/>
+        <v>99.5</v>
+      </c>
+      <c r="M10" s="7">
+        <f t="shared" si="1"/>
+        <v>150.4</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="P10" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D11" t="s">
         <v>21</v>
@@ -1158,8 +1288,8 @@
       <c r="E11">
         <v>19</v>
       </c>
-      <c r="F11" t="s">
-        <v>52</v>
+      <c r="F11" s="9" t="s">
+        <v>83</v>
       </c>
       <c r="G11">
         <v>333</v>
@@ -1168,7 +1298,7 @@
         <v>1126</v>
       </c>
       <c r="I11" t="s">
-        <v>53</v>
+        <v>87</v>
       </c>
       <c r="J11">
         <v>1</v>
@@ -1176,14 +1306,22 @@
       <c r="K11">
         <v>25</v>
       </c>
-      <c r="L11" t="s">
-        <v>54</v>
-      </c>
-      <c r="M11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L11" s="7">
+        <f t="shared" si="0"/>
+        <v>98.6</v>
+      </c>
+      <c r="M11" s="7">
+        <f t="shared" si="1"/>
+        <v>140</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="P11" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1191,15 +1329,15 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E12">
         <v>20</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="9" t="s">
         <v>18</v>
       </c>
       <c r="G12">
@@ -1217,14 +1355,22 @@
       <c r="K12">
         <v>35</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L12" s="7">
+        <f t="shared" si="0"/>
+        <v>3136.5</v>
+      </c>
+      <c r="M12" s="7">
+        <f t="shared" si="1"/>
+        <v>2344.8000000000002</v>
+      </c>
+      <c r="O12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="M12" t="s">
+      <c r="P12" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1232,15 +1378,15 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E13">
         <v>20</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="9" t="s">
         <v>18</v>
       </c>
       <c r="G13">
@@ -1250,7 +1396,7 @@
         <v>512</v>
       </c>
       <c r="I13" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="J13">
         <v>2</v>
@@ -1258,22 +1404,30 @@
       <c r="K13">
         <v>35</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L13" s="7">
+        <f t="shared" si="0"/>
+        <v>230.6</v>
+      </c>
+      <c r="M13" s="7">
+        <f t="shared" si="1"/>
+        <v>196.4</v>
+      </c>
+      <c r="O13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="M13" t="s">
+      <c r="P13" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="D14" t="s">
         <v>21</v>
@@ -1281,8 +1435,8 @@
       <c r="E14">
         <v>128</v>
       </c>
-      <c r="F14" t="s">
-        <v>58</v>
+      <c r="F14" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="G14">
         <v>200</v>
@@ -1291,7 +1445,7 @@
         <v>512</v>
       </c>
       <c r="I14" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="J14">
         <v>2</v>
@@ -1299,63 +1453,79 @@
       <c r="K14">
         <v>35</v>
       </c>
-      <c r="L14" t="s">
-        <v>75</v>
-      </c>
-      <c r="M14" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
+      <c r="L14" s="7">
+        <f t="shared" si="0"/>
+        <v>94.2</v>
+      </c>
+      <c r="M14" s="7">
+        <f t="shared" si="1"/>
+        <v>136.80000000000001</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="P14" s="12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" s="1" t="s">
+      <c r="B15" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="2">
         <v>156</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G15" s="1">
+      <c r="F15" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="2">
         <v>273</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15" s="2">
         <v>608</v>
       </c>
-      <c r="I15" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="J15" s="1">
+      <c r="I15" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J15" s="2">
         <v>2</v>
       </c>
-      <c r="K15" s="1">
+      <c r="K15" s="2">
         <v>45</v>
       </c>
-      <c r="L15" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L15" s="7">
+        <f t="shared" si="0"/>
+        <v>74.099999999999994</v>
+      </c>
+      <c r="M15" s="7">
+        <f t="shared" si="1"/>
+        <v>129.69999999999999</v>
+      </c>
+      <c r="O15" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="P15" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="C16" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="D16" t="s">
         <v>21</v>
@@ -1363,8 +1533,8 @@
       <c r="E16">
         <v>135</v>
       </c>
-      <c r="F16" t="s">
-        <v>58</v>
+      <c r="F16" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="G16">
         <v>202</v>
@@ -1373,7 +1543,7 @@
         <v>416</v>
       </c>
       <c r="I16" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="J16">
         <v>2</v>
@@ -1381,72 +1551,88 @@
       <c r="K16">
         <v>34</v>
       </c>
-      <c r="L16" t="s">
-        <v>83</v>
-      </c>
-      <c r="M16" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17">
+      <c r="L16" s="7">
+        <f t="shared" si="0"/>
+        <v>76.099999999999994</v>
+      </c>
+      <c r="M16" s="7">
+        <f t="shared" si="1"/>
+        <v>131</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="P16" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
-        <v>85</v>
-      </c>
-      <c r="C17" t="s">
-        <v>60</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="B17" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E17">
-        <v>89</v>
-      </c>
-      <c r="F17" t="s">
-        <v>58</v>
-      </c>
-      <c r="G17">
-        <v>293</v>
-      </c>
-      <c r="H17">
-        <v>384</v>
-      </c>
-      <c r="I17" t="s">
-        <v>86</v>
-      </c>
-      <c r="J17">
-        <v>2</v>
-      </c>
-      <c r="K17">
-        <v>45</v>
-      </c>
-      <c r="L17" t="s">
-        <v>87</v>
-      </c>
-      <c r="M17" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E17" s="1">
+        <v>128</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="G17" s="1">
+        <v>200</v>
+      </c>
+      <c r="H17" s="1">
+        <v>512</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J17" s="1">
+        <v>6</v>
+      </c>
+      <c r="K17" s="1">
+        <v>40</v>
+      </c>
+      <c r="L17" s="8">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="M17" s="8">
+        <f t="shared" si="1"/>
+        <v>120.5</v>
+      </c>
+      <c r="O17" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="P17" s="15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="D18" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E18">
         <v>128</v>
       </c>
-      <c r="F18" t="s">
-        <v>58</v>
+      <c r="F18" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="G18">
         <v>200</v>
@@ -1455,7 +1641,7 @@
         <v>512</v>
       </c>
       <c r="I18" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="J18">
         <v>6</v>
@@ -1463,31 +1649,39 @@
       <c r="K18">
         <v>35</v>
       </c>
-      <c r="L18" t="s">
-        <v>89</v>
-      </c>
-      <c r="M18" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L18" s="7">
+        <f t="shared" si="0"/>
+        <v>80.599999999999994</v>
+      </c>
+      <c r="M18" s="7">
+        <f t="shared" si="1"/>
+        <v>168.3</v>
+      </c>
+      <c r="O18" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="P18" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="D19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E19">
         <v>128</v>
       </c>
-      <c r="F19" t="s">
-        <v>58</v>
+      <c r="F19" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="G19">
         <v>200</v>
@@ -1496,7 +1690,7 @@
         <v>512</v>
       </c>
       <c r="I19" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="J19">
         <v>6</v>
@@ -1504,11 +1698,19 @@
       <c r="K19">
         <v>35</v>
       </c>
-      <c r="L19" t="s">
-        <v>91</v>
-      </c>
-      <c r="M19" t="s">
-        <v>92</v>
+      <c r="L19" s="7">
+        <f t="shared" si="0"/>
+        <v>57.8</v>
+      </c>
+      <c r="M19" s="7">
+        <f t="shared" si="1"/>
+        <v>147.9</v>
+      </c>
+      <c r="O19" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="P19" s="13" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>